<commit_message>
Commit code for WRN8NMB
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/8NMB_ConstructionCreation.xlsx
+++ b/src/test/resources/testdata/8NMB_ConstructionCreation.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="155">
   <si>
     <t>(Do Not Modify) Account</t>
   </si>
@@ -227,6 +227,279 @@
   </si>
   <si>
     <t>Projrefno_060924160913</t>
+  </si>
+  <si>
+    <t>Projrefno_090924045402</t>
+  </si>
+  <si>
+    <t>Projrefno_090924050109</t>
+  </si>
+  <si>
+    <t>Projrefno_090924050801</t>
+  </si>
+  <si>
+    <t>Projrefno_090924051113</t>
+  </si>
+  <si>
+    <t>Projrefno_090924051639</t>
+  </si>
+  <si>
+    <t>Projrefno_090924052336</t>
+  </si>
+  <si>
+    <t>Projrefno_090924055549</t>
+  </si>
+  <si>
+    <t>Projrefno_090924060424</t>
+  </si>
+  <si>
+    <t>Projrefno_090924113148</t>
+  </si>
+  <si>
+    <t>Projrefno_090924120346</t>
+  </si>
+  <si>
+    <t>Projrefno_100924044713</t>
+  </si>
+  <si>
+    <t>Projrefno_100924051711</t>
+  </si>
+  <si>
+    <t>Projrefno_100924053822</t>
+  </si>
+  <si>
+    <t>Projrefno_100924054605</t>
+  </si>
+  <si>
+    <t>Projrefno_100924055336</t>
+  </si>
+  <si>
+    <t>Projrefno_100924061218</t>
+  </si>
+  <si>
+    <t>Projrefno_100924063158</t>
+  </si>
+  <si>
+    <t>Projrefno_100924063417</t>
+  </si>
+  <si>
+    <t>Projrefno_100924064408</t>
+  </si>
+  <si>
+    <t>Projrefno_100924065434</t>
+  </si>
+  <si>
+    <t>Projrefno_100924070425</t>
+  </si>
+  <si>
+    <t>Projrefno_100924090207</t>
+  </si>
+  <si>
+    <t>Projrefno_100924114158</t>
+  </si>
+  <si>
+    <t>Projrefno_100924115601</t>
+  </si>
+  <si>
+    <t>Projrefno_100924121540</t>
+  </si>
+  <si>
+    <t>Projrefno_100924123247</t>
+  </si>
+  <si>
+    <t>Projrefno_100924160836</t>
+  </si>
+  <si>
+    <t>Projrefno_110924012055</t>
+  </si>
+  <si>
+    <t>Projrefno_110924013122</t>
+  </si>
+  <si>
+    <t>Projrefno_110924013534</t>
+  </si>
+  <si>
+    <t>Projrefno_110924014637</t>
+  </si>
+  <si>
+    <t>Projrefno_110924015607</t>
+  </si>
+  <si>
+    <t>Projrefno_110924040046</t>
+  </si>
+  <si>
+    <t>Projrefno_110924042445</t>
+  </si>
+  <si>
+    <t>Projrefno_110924043545</t>
+  </si>
+  <si>
+    <t>Projrefno_110924045850</t>
+  </si>
+  <si>
+    <t>Projrefno_110924054426</t>
+  </si>
+  <si>
+    <t>Projrefno_110924055357</t>
+  </si>
+  <si>
+    <t>Projrefno_110924061634</t>
+  </si>
+  <si>
+    <t>Projrefno_110924062713</t>
+  </si>
+  <si>
+    <t>Projrefno_110924063547</t>
+  </si>
+  <si>
+    <t>Projrefno_110924064801</t>
+  </si>
+  <si>
+    <t>Projrefno_110924065919</t>
+  </si>
+  <si>
+    <t>Projrefno_110924070203</t>
+  </si>
+  <si>
+    <t>Projrefno_110924090632</t>
+  </si>
+  <si>
+    <t>Projrefno_110924093344</t>
+  </si>
+  <si>
+    <t>Projrefno_110924094406</t>
+  </si>
+  <si>
+    <t>Projrefno_110924095901</t>
+  </si>
+  <si>
+    <t>Projrefno_110924101457</t>
+  </si>
+  <si>
+    <t>Projrefno_110924102720</t>
+  </si>
+  <si>
+    <t>Projrefno_110924111201</t>
+  </si>
+  <si>
+    <t>Projrefno_110924112000</t>
+  </si>
+  <si>
+    <t>Projrefno_110924115413</t>
+  </si>
+  <si>
+    <t>Projrefno_110924125105</t>
+  </si>
+  <si>
+    <t>Projrefno_110924131026</t>
+  </si>
+  <si>
+    <t>Projrefno_110924184423</t>
+  </si>
+  <si>
+    <t>Projrefno_110924184815</t>
+  </si>
+  <si>
+    <t>Projrefno_110924185749</t>
+  </si>
+  <si>
+    <t>Projrefno_110924192020</t>
+  </si>
+  <si>
+    <t>Projrefno_110924192256</t>
+  </si>
+  <si>
+    <t>Projrefno_110924192949</t>
+  </si>
+  <si>
+    <t>Projrefno_110924200409</t>
+  </si>
+  <si>
+    <t>Projrefno_110924205022</t>
+  </si>
+  <si>
+    <t>Projrefno_110924210659</t>
+  </si>
+  <si>
+    <t>DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>Projrefno_110924211333</t>
+  </si>
+  <si>
+    <t>Projrefno_120924055427</t>
+  </si>
+  <si>
+    <t>Projrefno_120924062148</t>
+  </si>
+  <si>
+    <t>Projrefno_120924062639</t>
+  </si>
+  <si>
+    <t>Projrefno_120924062900</t>
+  </si>
+  <si>
+    <t>Projrefno_120924063753</t>
+  </si>
+  <si>
+    <t>Projrefno_120924071708</t>
+  </si>
+  <si>
+    <t>Projrefno_120924085007</t>
+  </si>
+  <si>
+    <t>Projrefno_120924094556</t>
+  </si>
+  <si>
+    <t>Projrefno_120924095918</t>
+  </si>
+  <si>
+    <t>Projrefno_120924101334</t>
+  </si>
+  <si>
+    <t>Projrefno_120924102920</t>
+  </si>
+  <si>
+    <t>Projrefno_120924103712</t>
+  </si>
+  <si>
+    <t>Projrefno_120924104541</t>
+  </si>
+  <si>
+    <t>Projrefno_120924121037</t>
+  </si>
+  <si>
+    <t>Projrefno_120924121352</t>
+  </si>
+  <si>
+    <t>Projrefno_120924122555</t>
+  </si>
+  <si>
+    <t>Projrefno_120924123321</t>
+  </si>
+  <si>
+    <t>Projrefno_120924124309</t>
+  </si>
+  <si>
+    <t>Projrefno_120924125209</t>
+  </si>
+  <si>
+    <t>Projrefno_120924131628</t>
+  </si>
+  <si>
+    <t>Projrefno_120924154212</t>
+  </si>
+  <si>
+    <t>Projrefno_120924155333</t>
+  </si>
+  <si>
+    <t>Projrefno_120924155749</t>
+  </si>
+  <si>
+    <t>Projrefno_120924161655</t>
+  </si>
+  <si>
+    <t>Projrefno_120924163847</t>
   </si>
 </sst>
 </file>
@@ -695,7 +968,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="D2" s="5" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Anusha 0810 WRN4 started
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/8NMB_ConstructionCreation.xlsx
+++ b/src/test/resources/testdata/8NMB_ConstructionCreation.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="164">
   <si>
     <t>(Do Not Modify) Account</t>
   </si>
@@ -521,6 +521,12 @@
   </si>
   <si>
     <t>Projrefno_300924151825</t>
+  </si>
+  <si>
+    <t>Projrefno_041024102759</t>
+  </si>
+  <si>
+    <t>Projrefno_041024103859</t>
   </si>
 </sst>
 </file>
@@ -989,7 +995,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="D2" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>35</v>

</xml_diff>